<commit_message>
Evaluate values before parsing tests and add "enabled" parameter to Delete tag
</commit_message>
<xml_diff>
--- a/tests/Templates/delete_options.xlsx
+++ b/tests/Templates/delete_options.xlsx
@@ -219,6 +219,42 @@
   <si>
     <t>&amp;=if(Sheet1!A1="456","&lt;&lt;"&amp;"Delete&gt;&gt;","")&lt;&lt;OnlyValues&gt;&gt;</t>
   </si>
+  <si>
+    <t>&lt;&lt;delete enabled=true&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete enabled=no&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete enabled=false&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete enabled="false"&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete enabled={{enableCColumnDeletion}}&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete enabled={{enableEColumnDeletion}}&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disableCColumnDeletion={{enableCColumnDeletion}}&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disabled={{disableEColumnDeletion}}&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disabled={{disableCColumnDeletion}}&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disabled=""&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disabled=null&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disabled=&gt;&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -227,7 +263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="52" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -581,8 +617,22 @@
       <charset val="204"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <charset val="204"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Segoe UI"/>
+      <color rgb="FF000000"/>
+      <charset val="204"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,6 +682,9 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
       </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="none"/>
@@ -1175,7 +1228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="271">
+  <cellXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1831,6 +1884,10 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="50" applyFont="1" fillId="11" applyFill="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="51" applyFont="1" fillId="0" applyFill="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="50" applyFont="1" fillId="13" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="50" applyFont="1" fillId="14" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="52" applyFont="1" fillId="0" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="53" applyFont="1" fillId="0" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="49" applyFont="1" fillId="0" applyFill="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2323,7 +2380,7 @@
   <sheetViews>
     <sheetView showGridLines="false" tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScale="130" zoomScaleNormal="130">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9" activeCellId="0"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9" activeCellId="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2340,21 +2397,22 @@
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="11" customFormat="1" s="18">
+    <row r="1" customFormat="1" s="18">
       <c r="A1" s="269">
         <v>123</v>
       </c>
       <c r="B1" s="223" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="249"/>
+      <c r="C1" s="249" t="s">
+        <v>72</v>
+      </c>
       <c r="D1" s="224" t="s">
         <v>38</v>
       </c>
       <c r="E1" s="268" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
-      <c r="F1" s="148"/>
       <c r="H1" s="148"/>
       <c r="J1" s="148"/>
       <c r="K1" s="18"/>

</xml_diff>

<commit_message>
Add disabled parameter to "Delete" tag and evaluate values before parsing (#358)
* Evaluate values before parsing tests and add "enabled" parameter to Delete tag
</commit_message>
<xml_diff>
--- a/tests/Templates/delete_options.xlsx
+++ b/tests/Templates/delete_options.xlsx
@@ -219,6 +219,42 @@
   <si>
     <t>&amp;=if(Sheet1!A1="456","&lt;&lt;"&amp;"Delete&gt;&gt;","")&lt;&lt;OnlyValues&gt;&gt;</t>
   </si>
+  <si>
+    <t>&lt;&lt;delete enabled=true&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete enabled=no&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete enabled=false&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete enabled="false"&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete enabled={{enableCColumnDeletion}}&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete enabled={{enableEColumnDeletion}}&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disableCColumnDeletion={{enableCColumnDeletion}}&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disabled={{disableEColumnDeletion}}&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disabled={{disableCColumnDeletion}}&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disabled=""&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disabled=null&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;delete disabled=&gt;&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -227,7 +263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="52" x14ac:knownFonts="1">
+  <fonts count="54" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -581,8 +617,22 @@
       <charset val="204"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <charset val="204"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <name val="Segoe UI"/>
+      <color rgb="FF000000"/>
+      <charset val="204"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,6 +682,9 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
       </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="none"/>
@@ -1175,7 +1228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="271">
+  <cellXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1831,6 +1884,10 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="50" applyFont="1" fillId="11" applyFill="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="51" applyFont="1" fillId="0" applyFill="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="50" applyFont="1" fillId="13" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="50" applyFont="1" fillId="14" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="52" applyFont="1" fillId="0" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="53" applyFont="1" fillId="0" applyFill="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="49" applyFont="1" fillId="0" applyFill="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2323,7 +2380,7 @@
   <sheetViews>
     <sheetView showGridLines="false" tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScale="130" zoomScaleNormal="130">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9" activeCellId="0"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9" activeCellId="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2340,21 +2397,22 @@
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="11" customFormat="1" s="18">
+    <row r="1" customFormat="1" s="18">
       <c r="A1" s="269">
         <v>123</v>
       </c>
       <c r="B1" s="223" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="249"/>
+      <c r="C1" s="249" t="s">
+        <v>72</v>
+      </c>
       <c r="D1" s="224" t="s">
         <v>38</v>
       </c>
       <c r="E1" s="268" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
-      <c r="F1" s="148"/>
       <c r="H1" s="148"/>
       <c r="J1" s="148"/>
       <c r="K1" s="18"/>

</xml_diff>